<commit_message>
updated results for 12/11/24
</commit_message>
<xml_diff>
--- a/nba_predictor_results.xlsx
+++ b/nba_predictor_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shayl\Projects\nba_predictor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA05CC6-4D5B-4491-B7D7-045D72ACB90E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2D18F9-9F88-4E9C-8A7A-A005E509B368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{7CC4E96F-BD3B-46E8-AC91-3EE34230F958}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="65">
   <si>
     <t>Date</t>
   </si>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t>Overs, L10 Games</t>
+  </si>
+  <si>
+    <t>Warriors +2.5</t>
   </si>
 </sst>
 </file>
@@ -632,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A559E30-137E-4836-8835-F7B14D3C49F3}">
-  <dimension ref="A1:R33"/>
+  <dimension ref="A1:R34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -754,11 +757,11 @@
       </c>
       <c r="G3" s="5">
         <f>SUM(F:F)</f>
-        <v>5.454545454545455</v>
+        <v>4.454545454545455</v>
       </c>
       <c r="H3" s="4" t="str">
         <f>COUNTIF(E:E,"W") &amp;"-" &amp;COUNTIF(E:E,"L")</f>
-        <v>17-10</v>
+        <v>17-11</v>
       </c>
       <c r="J3" s="1">
         <v>45617</v>
@@ -784,11 +787,11 @@
       </c>
       <c r="Q3" s="5">
         <f>SUM(P:P)</f>
-        <v>1.1214814814814811</v>
+        <v>2.0305723905723903</v>
       </c>
       <c r="R3" s="4" t="str">
         <f>COUNTIF(O:O,"W") &amp;"-" &amp;COUNTIF(O:O,"L")</f>
-        <v>15-16</v>
+        <v>16-16</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
@@ -831,7 +834,7 @@
         <v>14</v>
       </c>
       <c r="P4" s="2">
-        <f t="shared" ref="P4:P33" si="0">IF(O4="L",-1,IF(N4&lt;0,1/(-N4/100),1*(N4/100)))</f>
+        <f t="shared" ref="P4:P34" si="0">IF(O4="L",-1,IF(N4&lt;0,1/(-N4/100),1*(N4/100)))</f>
         <v>2.25</v>
       </c>
     </row>
@@ -852,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" ref="F5:F29" si="1">IF(E5="L",-1,IF(E5="W",1/1.1,0))</f>
+        <f t="shared" ref="F5:F30" si="1">IF(E5="L",-1,IF(E5="W",1/1.1,0))</f>
         <v>0.90909090909090906</v>
       </c>
       <c r="G5" s="2"/>
@@ -1933,6 +1936,25 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>45637</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="6">
+        <v>237.5</v>
+      </c>
+      <c r="E30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30" s="2">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
       <c r="J30" s="1">
         <v>45631</v>
       </c>
@@ -2024,6 +2046,30 @@
         <v>14</v>
       </c>
       <c r="P33" s="2">
+        <f t="shared" si="0"/>
+        <v>0.90909090909090906</v>
+      </c>
+    </row>
+    <row r="34" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J34" s="1">
+        <v>45637</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M34" t="s">
+        <v>64</v>
+      </c>
+      <c r="N34">
+        <v>-110</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P34" s="2">
         <f t="shared" si="0"/>
         <v>0.90909090909090906</v>
       </c>

</xml_diff>

<commit_message>
updated results for 12/13/24
</commit_message>
<xml_diff>
--- a/nba_predictor_results.xlsx
+++ b/nba_predictor_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shayl\Projects\nba_predictor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2D18F9-9F88-4E9C-8A7A-A005E509B368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8996BDA6-8591-473A-9287-D822AE69813A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{7CC4E96F-BD3B-46E8-AC91-3EE34230F958}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="66">
   <si>
     <t>Date</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>Warriors +2.5</t>
+  </si>
+  <si>
+    <t>Trail Blazers</t>
   </si>
 </sst>
 </file>
@@ -635,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A559E30-137E-4836-8835-F7B14D3C49F3}">
-  <dimension ref="A1:R34"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -757,11 +760,11 @@
       </c>
       <c r="G3" s="5">
         <f>SUM(F:F)</f>
-        <v>4.454545454545455</v>
+        <v>4.3636363636363642</v>
       </c>
       <c r="H3" s="4" t="str">
         <f>COUNTIF(E:E,"W") &amp;"-" &amp;COUNTIF(E:E,"L")</f>
-        <v>17-11</v>
+        <v>18-12</v>
       </c>
       <c r="J3" s="1">
         <v>45617</v>
@@ -787,11 +790,11 @@
       </c>
       <c r="Q3" s="5">
         <f>SUM(P:P)</f>
-        <v>2.0305723905723903</v>
+        <v>2.6555723905723903</v>
       </c>
       <c r="R3" s="4" t="str">
         <f>COUNTIF(O:O,"W") &amp;"-" &amp;COUNTIF(O:O,"L")</f>
-        <v>16-16</v>
+        <v>17-16</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
@@ -834,7 +837,7 @@
         <v>14</v>
       </c>
       <c r="P4" s="2">
-        <f t="shared" ref="P4:P34" si="0">IF(O4="L",-1,IF(N4&lt;0,1/(-N4/100),1*(N4/100)))</f>
+        <f t="shared" ref="P4:P35" si="0">IF(O4="L",-1,IF(N4&lt;0,1/(-N4/100),1*(N4/100)))</f>
         <v>2.25</v>
       </c>
     </row>
@@ -855,7 +858,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" ref="F5:F30" si="1">IF(E5="L",-1,IF(E5="W",1/1.1,0))</f>
+        <f t="shared" ref="F5:F32" si="1">IF(E5="L",-1,IF(E5="W",1/1.1,0))</f>
         <v>0.90909090909090906</v>
       </c>
       <c r="G5" s="2"/>
@@ -1979,6 +1982,25 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>45639</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="6">
+        <v>232.5</v>
+      </c>
+      <c r="E31" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
       <c r="J31" s="1">
         <v>45631</v>
       </c>
@@ -2003,6 +2025,25 @@
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>45640</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="6">
+        <v>228.5</v>
+      </c>
+      <c r="E32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="2">
+        <f t="shared" si="1"/>
+        <v>0.90909090909090906</v>
+      </c>
       <c r="J32" s="1">
         <v>45632</v>
       </c>
@@ -2072,6 +2113,30 @@
       <c r="P34" s="2">
         <f t="shared" si="0"/>
         <v>0.90909090909090906</v>
+      </c>
+    </row>
+    <row r="35" spans="10:16" x14ac:dyDescent="0.3">
+      <c r="J35" s="1">
+        <v>45639</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M35" t="s">
+        <v>52</v>
+      </c>
+      <c r="N35">
+        <v>-160</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P35" s="2">
+        <f t="shared" si="0"/>
+        <v>0.625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>